<commit_message>
添加R6250H0整机与openEuler 20.03 LTS SP4适配结果
</commit_message>
<xml_diff>
--- a/data/compatibility/openEuler22.03-LTS-SP2上两类平台板卡兼容清单.xlsx
+++ b/data/compatibility/openEuler22.03-LTS-SP2上两类平台板卡兼容清单.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="135">
   <si>
     <t>vendorID</t>
   </si>
@@ -582,6 +582,45 @@
   </si>
   <si>
     <t>02311LSY</t>
+  </si>
+  <si>
+    <t>1ec6</t>
+  </si>
+  <si>
+    <t>0200</t>
+  </si>
+  <si>
+    <t>0063</t>
+  </si>
+  <si>
+    <t>vastai_pci</t>
+  </si>
+  <si>
+    <t>CD9440DD8E1973C48A18416</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>2024.1.19</t>
+  </si>
+  <si>
+    <t>df47d49f3418d5a61002739a246470d35238c8bff4d4ee2fa1081c186c95bf57</t>
+  </si>
+  <si>
+    <t>29.8M</t>
+  </si>
+  <si>
+    <t>VASTAI</t>
+  </si>
+  <si>
+    <t>VG1000</t>
+  </si>
+  <si>
+    <t>SG100</t>
+  </si>
+  <si>
+    <t>https://repo.oepkgs.net/openEuler/rpm/openEuler-22.03-LTS-SP2/contrib/drivers/source/Packages/ddk_pack.tar.gz</t>
   </si>
   <si>
     <t>板卡</t>
@@ -1717,12 +1756,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
+      <selection pane="bottomLeft" activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3899,6 +3938,56 @@
       </c>
       <c r="Q42" s="6" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="N43" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q43" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3954,10 +4043,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" ht="27" customHeight="1"/>

</xml_diff>